<commit_message>
Add 5 more lab results
</commit_message>
<xml_diff>
--- a/input/vocabulary/spreadsheets/1_Comprehensive_Metabolic_Panel.xlsx
+++ b/input/vocabulary/spreadsheets/1_Comprehensive_Metabolic_Panel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dcarlson/git/chronic-care/covidml-cql/input/vocabulary/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01D4BD5D-FAD1-8A4C-A7FE-4C1B8A652C41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2127192C-1453-7046-8213-784A543C5FA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -355,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -371,6 +371,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,11 +926,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F40"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="12" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+      <selection pane="bottomLeft" activeCell="A13" sqref="A13:XFD13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -994,7 +997,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
@@ -1015,25 +1018,19 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="7"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>2</v>
@@ -1044,10 +1041,10 @@
     </row>
     <row r="15" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>2</v>
@@ -1058,10 +1055,10 @@
     </row>
     <row r="16" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>2</v>
@@ -1070,177 +1067,180 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="18" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="C18" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="C19" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="C20" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C20" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B22" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C21" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="C22" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B23" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C22" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="C23" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B24" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C23" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="31" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="C24" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="31" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="C25" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="C26" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="C27" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C27" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="C28" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C28" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="C29" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C29" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="C30" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B31" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="C31" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B32" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="4" t="s">
-        <v>60</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>2</v>
@@ -1248,10 +1248,10 @@
     </row>
     <row r="33" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>2</v>
@@ -1259,10 +1259,10 @@
     </row>
     <row r="34" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>2</v>
@@ -1270,10 +1270,10 @@
     </row>
     <row r="35" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>2</v>
@@ -1281,10 +1281,10 @@
     </row>
     <row r="36" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>2</v>
@@ -1292,10 +1292,10 @@
     </row>
     <row r="37" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>2</v>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="38" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>2</v>
@@ -1314,10 +1314,10 @@
     </row>
     <row r="39" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>2</v>
@@ -1325,12 +1325,23 @@
     </row>
     <row r="40" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B41" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C41" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>